<commit_message>
table plus database exports excel_pdf_deletenig etc
</commit_message>
<xml_diff>
--- a/exports/orders_export.xlsx
+++ b/exports/orders_export.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -487,16 +487,16 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>ORD001</t>
+          <t>ORD014</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Lukas Krumpach</t>
+          <t>Hana VAVROVA</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -506,7 +506,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Premonstrátů 910C</t>
+          <t>Jaktáře 1475</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -519,12 +519,12 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>2025-03-23</t>
+          <t>2025-03-25</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>F001</t>
+          <t>F014</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -535,11 +535,11 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ORD002</t>
+          <t>ORD013</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -567,42 +567,42 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>2025-03-23</t>
+          <t>2025-03-25</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>F002</t>
+          <t>F013</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Nová</t>
+          <t>Zpracovává se</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>ORD003</t>
+          <t>ORD012</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Lukas Krumpach</t>
+          <t>Mariia Isova</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>lukas.krumpach@gmail.com</t>
+          <t>l.m.e.companycz@gmail.com</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Premonstrátů 910C</t>
+          <t>Názovská 14</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -615,12 +615,12 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>2025-03-23</t>
+          <t>2025-03-24</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>F003</t>
+          <t>F012</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
@@ -631,16 +631,16 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>ORD004</t>
+          <t>ORD011</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Lukas Krumpach</t>
+          <t>Лукас Крумпах</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -650,7 +650,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Premonstrátů 910C</t>
+          <t>Moscow, Потаповский переулок, д. 8/12 стр. 2</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -663,12 +663,12 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>2025-03-23</t>
+          <t>2025-03-24</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>F004</t>
+          <t>F011</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
@@ -679,16 +679,16 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>ORD005</t>
+          <t>ORD010</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Лукас Крумпах</t>
+          <t>Lukas Krumpach</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -698,7 +698,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Moscow, Потаповский переулок, д. 8/12 стр. 2</t>
+          <t>Premonstrátů 910C</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -711,12 +711,12 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>2025-03-23</t>
+          <t>2025-03-24</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>F005</t>
+          <t>F010</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
@@ -727,11 +727,11 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>ORD006</t>
+          <t>ORD009</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -759,12 +759,12 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>2025-03-23</t>
+          <t>2025-03-24</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>F006</t>
+          <t>F009</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
@@ -775,11 +775,11 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>ORD007</t>
+          <t>ORD008</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -812,7 +812,7 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>F007</t>
+          <t>F008</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
@@ -823,11 +823,11 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>ORD008</t>
+          <t>ORD007</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -860,10 +860,298 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>F008</t>
+          <t>F007</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
+        <is>
+          <t>Nová</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>6</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>ORD006</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Lukas Krumpach</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>lukas.krumpach@gmail.com</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Premonstrátů 910C</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>🔥 HYALCHONDRO® HC PLUS</t>
+        </is>
+      </c>
+      <c r="G10" t="n">
+        <v>1</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>2025-03-23</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>F006</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>Nová</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>5</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>ORD005</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Лукас Крумпах</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>lukas.krumpach@gmail.com</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Moscow, Потаповский переулок, д. 8/12 стр. 2</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>🔥 HYALCHONDRO® HC PLUS</t>
+        </is>
+      </c>
+      <c r="G11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>2025-03-23</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>F005</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>Nová</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>4</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>ORD004</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Lukas Krumpach</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>lukas.krumpach@gmail.com</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Premonstrátů 910C</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>🔥 HYALCHONDRO® HC PLUS</t>
+        </is>
+      </c>
+      <c r="G12" t="n">
+        <v>1</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>2025-03-23</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>F004</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>Nová</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>3</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>ORD003</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Lukas Krumpach</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>lukas.krumpach@gmail.com</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Premonstrátů 910C</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>🔥 HYALCHONDRO® HC PLUS</t>
+        </is>
+      </c>
+      <c r="G13" t="n">
+        <v>1</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>2025-03-23</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>F003</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>Nová</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>2</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>ORD002</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Лукас Крумпах</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>lukas.krumpach@gmail.com</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Moscow, Потаповский переулок, д. 8/12 стр. 2</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>🔥 HYALCHONDRO® HC PLUS</t>
+        </is>
+      </c>
+      <c r="G14" t="n">
+        <v>1</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>2025-03-23</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>F002</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>Nová</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>1</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>ORD001</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Lukas Krumpach</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>lukas.krumpach@gmail.com</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Premonstrátů 910C</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>🔥 HYALCHONDRO® HC PLUS</t>
+        </is>
+      </c>
+      <c r="G15" t="n">
+        <v>1</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>2025-03-23</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>F001</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
         <is>
           <t>Nová</t>
         </is>

</xml_diff>

<commit_message>
chatbot and telegram db
</commit_message>
<xml_diff>
--- a/exports/orders_export.xlsx
+++ b/exports/orders_export.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -487,16 +487,16 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>ORD014</t>
+          <t>ORD020</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Hana VAVROVA</t>
+          <t>Лукас Крумпах</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -506,7 +506,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Jaktáře 1475</t>
+          <t>Moscow, Потаповский переулок, д. 8/12 стр. 2</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -519,12 +519,12 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>2025-03-25</t>
+          <t>2025-03-26</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>F014</t>
+          <t>F020</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -535,11 +535,11 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ORD013</t>
+          <t>ORD019</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -572,7 +572,7 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>F013</t>
+          <t>F019</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
@@ -583,26 +583,26 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>ORD012</t>
+          <t>ORD018</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Mariia Isova</t>
+          <t>Hana VAVROVA</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>l.m.e.companycz@gmail.com</t>
+          <t>lukas.krumpach@gmail.com</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Názovská 14</t>
+          <t>Jaktáře 14756666666666666666666666</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -615,12 +615,12 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-25</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>F012</t>
+          <t>F018</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
@@ -631,16 +631,16 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>ORD011</t>
+          <t>ORD017</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Лукас Крумпах</t>
+          <t>Lukas Krumpach</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -650,7 +650,8 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Moscow, Потаповский переулок, д. 8/12 стр. 2</t>
+          <t>Pod Lipami
+C.P. 24 44444444444444444444</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -663,12 +664,12 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-25</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>F011</t>
+          <t>F017</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
@@ -679,16 +680,16 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>ORD010</t>
+          <t>ORD016</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Lukas Krumpach</t>
+          <t>Hana VAVROVA</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -698,7 +699,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Premonstrátů 910C</t>
+          <t>Jaktáře 1475 3333333333333333333</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -711,12 +712,12 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-25</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>F010</t>
+          <t>F016</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
@@ -727,11 +728,11 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>ORD009</t>
+          <t>ORD015</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -746,7 +747,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Premonstrátů 910C</t>
+          <t>Premonstrátů 910C 22222222222222222222222222222</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -759,32 +760,32 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-25</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>F009</t>
+          <t>F015</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>Nová</t>
+          <t>Odesláno</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>ORD008</t>
+          <t>ORD014</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Lukas Krumpach</t>
+          <t>Hana VAVROVA</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -794,7 +795,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Premonstrátů 910C</t>
+          <t>Jaktáře 1475</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -807,12 +808,12 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>2025-03-23</t>
+          <t>2025-03-25</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>F008</t>
+          <t>F014</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
@@ -823,16 +824,16 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>ORD007</t>
+          <t>ORD013</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Lukas Krumpach</t>
+          <t>Лукас Крумпах</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -842,7 +843,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Premonstrátů 910C</t>
+          <t>Moscow, Потаповский переулок, д. 8/12 стр. 2</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -855,42 +856,42 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>2025-03-23</t>
+          <t>2025-03-25</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>F007</t>
+          <t>F013</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>Nová</t>
+          <t>Zpracovává se</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>ORD006</t>
+          <t>ORD012</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Lukas Krumpach</t>
+          <t>Mariia Isova</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>lukas.krumpach@gmail.com</t>
+          <t>l.m.e.companycz@gmail.com</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Premonstrátů 910C</t>
+          <t>Názovská 14</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -903,12 +904,12 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>2025-03-23</t>
+          <t>2025-03-24</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>F006</t>
+          <t>F012</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
@@ -919,11 +920,11 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>ORD005</t>
+          <t>ORD011</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -951,12 +952,12 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>2025-03-23</t>
+          <t>2025-03-24</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>F005</t>
+          <t>F011</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
@@ -967,11 +968,11 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>ORD004</t>
+          <t>ORD010</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -999,12 +1000,12 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>2025-03-23</t>
+          <t>2025-03-24</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>F004</t>
+          <t>F010</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
@@ -1015,11 +1016,11 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>ORD003</t>
+          <t>ORD009</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -1047,12 +1048,12 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>2025-03-23</t>
+          <t>2025-03-24</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>F003</t>
+          <t>F009</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
@@ -1063,16 +1064,16 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>ORD002</t>
+          <t>ORD008</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Лукас Крумпах</t>
+          <t>Lukas Krumpach</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -1082,7 +1083,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Moscow, Потаповский переулок, д. 8/12 стр. 2</t>
+          <t>Premonstrátů 910C</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1100,7 +1101,7 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>F002</t>
+          <t>F008</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
@@ -1111,47 +1112,335 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
+          <t>ORD007</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Lukas Krumpach</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>lukas.krumpach@gmail.com</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Premonstrátů 910C</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>🔥 HYALCHONDRO® HC PLUS</t>
+        </is>
+      </c>
+      <c r="G15" t="n">
+        <v>1</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>2025-03-23</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>F007</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>Nová</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>6</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>ORD006</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Lukas Krumpach</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>lukas.krumpach@gmail.com</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Premonstrátů 910C</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>🔥 HYALCHONDRO® HC PLUS</t>
+        </is>
+      </c>
+      <c r="G16" t="n">
+        <v>1</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>2025-03-23</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>F006</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>Nová</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>5</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>ORD005</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Лукас Крумпах</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>lukas.krumpach@gmail.com</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Moscow, Потаповский переулок, д. 8/12 стр. 2</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>🔥 HYALCHONDRO® HC PLUS</t>
+        </is>
+      </c>
+      <c r="G17" t="n">
+        <v>1</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>2025-03-23</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>F005</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>Nová</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>4</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>ORD004</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Lukas Krumpach</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>lukas.krumpach@gmail.com</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Premonstrátů 910C</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>🔥 HYALCHONDRO® HC PLUS</t>
+        </is>
+      </c>
+      <c r="G18" t="n">
+        <v>1</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>2025-03-23</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>F004</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>Nová</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>3</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>ORD003</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Lukas Krumpach</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>lukas.krumpach@gmail.com</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Premonstrátů 910C</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>🔥 HYALCHONDRO® HC PLUS</t>
+        </is>
+      </c>
+      <c r="G19" t="n">
+        <v>1</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>2025-03-23</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>F003</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>Nová</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>2</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>ORD002</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Лукас Крумпах</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>lukas.krumpach@gmail.com</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Moscow, Потаповский переулок, д. 8/12 стр. 2</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>🔥 HYALCHONDRO® HC PLUS</t>
+        </is>
+      </c>
+      <c r="G20" t="n">
+        <v>1</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>2025-03-23</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>F002</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>Nová</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>1</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
           <t>ORD001</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="C21" t="inlineStr">
         <is>
           <t>Lukas Krumpach</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>lukas.krumpach@gmail.com</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>lukas.krumpach@gmail.com</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
         <is>
           <t>Premonstrátů 910C</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>🔥 HYALCHONDRO® HC PLUS</t>
-        </is>
-      </c>
-      <c r="G15" t="n">
-        <v>1</v>
-      </c>
-      <c r="H15" t="inlineStr">
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>🔥 HYALCHONDRO® HC PLUS</t>
+        </is>
+      </c>
+      <c r="G21" t="n">
+        <v>1</v>
+      </c>
+      <c r="H21" t="inlineStr">
         <is>
           <t>2025-03-23</t>
         </is>
       </c>
-      <c r="I15" t="inlineStr">
+      <c r="I21" t="inlineStr">
         <is>
           <t>F001</t>
         </is>
       </c>
-      <c r="J15" t="inlineStr">
+      <c r="J21" t="inlineStr">
         <is>
           <t>Nová</t>
         </is>

</xml_diff>